<commit_message>
Fix: edit extraction code to have correct fields
</commit_message>
<xml_diff>
--- a/data/audit/Audit.xlsx
+++ b/data/audit/Audit.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,15 +436,20 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>audit_id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>name</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>type</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>major</t>
         </is>
@@ -453,13 +458,18 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>is_0</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>BS in Information Systems</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>0</v>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>is</t>
         </is>
@@ -468,13 +478,18 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>is_1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>GenEd</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>1</v>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>is</t>
         </is>
@@ -483,13 +498,18 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>cs_0</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>BS in Computer Science</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>0</v>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>cs</t>
         </is>
@@ -498,13 +518,18 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>cs_1</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>GenEd</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>1</v>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>cs</t>
         </is>
@@ -513,13 +538,18 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>ba_0</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>BS in Business Administration</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>0</v>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>ba</t>
         </is>
@@ -528,13 +558,18 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>ba_1</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>EY2022 Qatar Business Administration - University Core Requirements</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="C7" t="n">
         <v>1</v>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>ba</t>
         </is>
@@ -543,13 +578,18 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>bs_0</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>BS in Biological Sciences</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="C8" t="n">
         <v>0</v>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>bs</t>
         </is>
@@ -558,13 +598,18 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>bs_1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>GenEd</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="C9" t="n">
         <v>1</v>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>bs</t>
         </is>

</xml_diff>

<commit_message>
Fix: changed formatting to be uniform and pass pylint
</commit_message>
<xml_diff>
--- a/data/audit/Audit.xlsx
+++ b/data/audit/Audit.xlsx
@@ -436,182 +436,182 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>major</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>audit_id</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>major</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>BS in Information Systems</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>is</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>is_0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>BS in Information Systems</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>is</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>GenEd</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>is</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>is_1</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>GenEd</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>is</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>BS in Computer Science</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>cs</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>cs_0</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>BS in Computer Science</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>cs</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>GenEd</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>cs</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>cs_1</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>GenEd</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>cs</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>BS in Business Administration</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>ba</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>ba_0</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>BS in Business Administration</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>ba</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>EY2022 Qatar Business Administration - University Core Requirements</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>ba</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>ba_1</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>EY2022 Qatar Business Administration - University Core Requirements</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>ba</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>BS in Biological Sciences</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>bs</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>bs_0</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>BS in Biological Sciences</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>bs</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>GenEd</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>bs</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
           <t>bs_1</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>GenEd</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>bs</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update: changed audit jsons provided by prof Giselle
</commit_message>
<xml_diff>
--- a/data/audit/Audit.xlsx
+++ b/data/audit/Audit.xlsx
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BS in Information Systems</t>
+          <t>BS in Biological Sciences</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -466,12 +466,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>is</t>
+          <t>bio</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>is_0</t>
+          <t>bio_0</t>
         </is>
       </c>
     </row>
@@ -486,19 +486,19 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>is</t>
+          <t>bio</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>is_1</t>
+          <t>bio_1</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>BS in Computer Science</t>
+          <t>BS in Information Systems</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,12 +506,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>cs</t>
+          <t>is</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>cs_0</t>
+          <t>is_0</t>
         </is>
       </c>
     </row>
@@ -526,19 +526,19 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>cs</t>
+          <t>is</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>cs_1</t>
+          <t>is_1</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>BS in Business Administration</t>
+          <t>BS in Computer Science</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -546,19 +546,19 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ba</t>
+          <t>cs</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>ba_0</t>
+          <t>cs_0</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>EY2022 Qatar Business Administration - University Core Requirements</t>
+          <t>GenEd</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -566,19 +566,19 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ba</t>
+          <t>cs</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>ba_1</t>
+          <t>cs_1</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>BS in Biological Sciences</t>
+          <t>BS in Business Administration</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -586,19 +586,19 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>bs</t>
+          <t>ba</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>bs_0</t>
+          <t>ba_0</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>GenEd</t>
+          <t>EY2022 Qatar Business Administration - University Core Requirements</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -606,12 +606,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>bs</t>
+          <t>ba</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>bs_1</t>
+          <t>ba_1</t>
         </is>
       </c>
     </row>

</xml_diff>